<commit_message>
Fuel Information update with Default Efficiency.
</commit_message>
<xml_diff>
--- a/data/Fuel.xlsx
+++ b/data/Fuel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>btus</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>price_col</t>
+  </si>
+  <si>
+    <t>effic</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -191,6 +194,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -530,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,12 +546,12 @@
     <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -563,11 +567,14 @@
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -583,11 +590,14 @@
       <c r="E2" s="5">
         <v>117</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -603,11 +613,14 @@
       <c r="E3" s="5">
         <v>139</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -623,11 +636,14 @@
       <c r="E4" s="5">
         <v>161.30000000000001</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -643,11 +659,14 @@
       <c r="E5" s="5">
         <v>161.30000000000001</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -663,11 +682,14 @@
       <c r="E6" s="5">
         <v>0</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="8">
+        <v>0.63</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -683,11 +705,14 @@
       <c r="E7" s="5">
         <v>0</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="8">
+        <v>0.63</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -703,11 +728,14 @@
       <c r="E8" s="5">
         <v>214.3</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="8">
+        <v>0.63</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -723,11 +751,14 @@
       <c r="E9" s="5">
         <v>58</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="8">
+        <v>0.99</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -743,7 +774,10 @@
       <c r="E10" s="5">
         <v>58</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="8">
+        <v>0.99</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>